<commit_message>
Add a partial readme
</commit_message>
<xml_diff>
--- a/Stadistics.xlsx
+++ b/Stadistics.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="28">
   <si>
     <t>Team</t>
   </si>
@@ -512,7 +512,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,7 +981,9 @@
       <c r="G17" s="2">
         <v>2</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="I17" s="7" t="s">
         <v>26</v>
       </c>
@@ -1008,7 +1010,9 @@
       <c r="G18" s="2">
         <v>17</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="I18" s="2" t="s">
         <v>27</v>
       </c>
@@ -1062,7 +1066,9 @@
       <c r="G20" s="2">
         <v>3</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="I20" s="7" t="s">
         <v>26</v>
       </c>
@@ -1089,7 +1095,9 @@
       <c r="G21" s="2">
         <v>4</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="I21" s="2" t="s">
         <v>27</v>
       </c>
@@ -1208,11 +1216,15 @@
       <c r="C27" s="2">
         <v>108574574</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2">
+        <v>4</v>
+      </c>
       <c r="E27" s="2">
         <v>1</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="2">
+        <v>3</v>
+      </c>
       <c r="G27" s="2">
         <v>2</v>
       </c>
@@ -1229,11 +1241,15 @@
       <c r="C28" s="3">
         <v>90738581</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2">
+        <v>7</v>
+      </c>
       <c r="E28" s="2">
         <v>0</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="2">
+        <v>2</v>
+      </c>
       <c r="G28" s="2">
         <v>17</v>
       </c>
@@ -1271,11 +1287,15 @@
       <c r="C30" s="2">
         <v>127511146</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2">
+        <v>6</v>
+      </c>
       <c r="E30" s="2">
         <v>1</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="2">
+        <v>4</v>
+      </c>
       <c r="G30" s="2">
         <v>3</v>
       </c>
@@ -1292,11 +1312,15 @@
       <c r="C31" s="2">
         <v>108699969</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <v>7</v>
+      </c>
       <c r="E31" s="2">
         <v>0</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
       <c r="G31" s="2">
         <v>4</v>
       </c>

</xml_diff>